<commit_message>
Updated Invoice Modules script need to update once Bug fixed
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Invoice.data.xlsx
+++ b/tests/artifact/data/UI-Invoice.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="252">
   <si>
     <t>login.screen</t>
   </si>
@@ -945,19 +945,19 @@
     <t>print.original</t>
   </si>
   <si>
-    <t>//div[@id='triplicate-wrapper']/button/span[text()='Original']</t>
+    <t>//button/span[text()='Original']</t>
   </si>
   <si>
     <t>print.duplicate</t>
   </si>
   <si>
-    <t>//div[@id='triplicate-wrapper']/button/span[text()='Duplicate']</t>
+    <t>//button/span[text()='Duplicate']</t>
   </si>
   <si>
     <t>print.triplicate</t>
   </si>
   <si>
-    <t>//div[@id='triplicate-wrapper']/button/span[text()='Triplicate']</t>
+    <t>//button/span[text()='Triplicate']</t>
   </si>
   <si>
     <t>invoice.popup.message</t>
@@ -990,10 +990,55 @@
     <t>//*[@id='list-Invoice']/tbody/tr/td[2]</t>
   </si>
   <si>
-    <t>invoice</t>
-  </si>
-  <si>
-    <t>//div</t>
+    <t>buyerDetails.Name</t>
+  </si>
+  <si>
+    <t>(//div[@class='card-body'])[3]/p/span[1]</t>
+  </si>
+  <si>
+    <t>Print.button</t>
+  </si>
+  <si>
+    <t>//div[@class='card ml-md-2']/div/div/button</t>
+  </si>
+  <si>
+    <t>bd.supplier.name</t>
+  </si>
+  <si>
+    <t>VEGAN COCONUT MILK POWDER</t>
+  </si>
+  <si>
+    <t>bd.edit.supplier.address</t>
+  </si>
+  <si>
+    <t>R-102, 1st Floor, TTC Industrial Estate, MIDC Rabale, Navi Mumbai - 400701</t>
+  </si>
+  <si>
+    <t>bd.edit.supplier.pincode</t>
+  </si>
+  <si>
+    <t>bd.edit.supplier.state</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>bd.edit.supplier.GSTIN</t>
+  </si>
+  <si>
+    <t>29AAQFA1638Q1ZP</t>
+  </si>
+  <si>
+    <t>attachment.file.path</t>
+  </si>
+  <si>
+    <t>C:\Projects\GNU\GNUKhata\artifact\data/InvoiceAttachment.pdf</t>
+  </si>
+  <si>
+    <t>Item.select.values</t>
+  </si>
+  <si>
+    <t>CreateItem</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1051,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1045,6 +1090,12 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11.25"/>
+      <color rgb="FF0B5E4E"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1519,152 +1570,152 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1699,6 +1750,9 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2113,8 +2167,8 @@
   <sheetPr/>
   <dimension ref="A1:B208"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -3071,44 +3125,76 @@
       </c>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="4"/>
-      <c r="B119" s="5"/>
+      <c r="A119" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="4"/>
-      <c r="B121" s="5"/>
+      <c r="A121" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="4"/>
-      <c r="B122" s="5"/>
+      <c r="A122" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="4"/>
-      <c r="B123" s="5"/>
+      <c r="A123" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B123" s="9">
+        <v>400701</v>
+      </c>
     </row>
     <row r="124" spans="1:2">
-      <c r="A124" s="4"/>
-      <c r="B124" s="5"/>
+      <c r="A124" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="4"/>
-      <c r="B125" s="5"/>
+      <c r="A125" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="4"/>
-      <c r="B126" s="5"/>
+      <c r="A126" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="4"/>
-      <c r="B127" s="5"/>
+      <c r="A127" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="4"/>

</xml_diff>

<commit_message>
Updated Invoice Module Need to be updated again once Bugs are fixed
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Invoice.data.xlsx
+++ b/tests/artifact/data/UI-Invoice.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="250">
   <si>
     <t>login.screen</t>
   </si>
@@ -1033,12 +1033,6 @@
   </si>
   <si>
     <t>C:\Projects\GNU\GNUKhata\artifact\data/InvoiceAttachment.pdf</t>
-  </si>
-  <si>
-    <t>Item.select.values</t>
-  </si>
-  <si>
-    <t>CreateItem</t>
   </si>
 </sst>
 </file>
@@ -2165,7 +2159,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B208"/>
+  <dimension ref="A1:B207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A115" workbookViewId="0">
       <selection activeCell="A128" sqref="A128"/>
@@ -3189,12 +3183,8 @@
       </c>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>251</v>
-      </c>
+      <c r="A127" s="4"/>
+      <c r="B127" s="5"/>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="4"/>
@@ -3515,10 +3505,6 @@
     <row r="207" spans="1:2">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
-    </row>
-    <row r="208" spans="1:2">
-      <c r="A208" s="4"/>
-      <c r="B208" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>

</xml_diff>

<commit_message>
Updated script as per the page updation
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-Invoice.data.xlsx
+++ b/tests/artifact/data/UI-Invoice.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="303">
   <si>
     <t>login.screen</t>
   </si>
@@ -196,7 +196,7 @@
     <t>org.open</t>
   </si>
   <si>
-    <t>(//button[text()=' Open '])[108]</t>
+    <t>(//button[text()=' Open '])[104]</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -238,13 +238,13 @@
     <t>ci.SaleButton</t>
   </si>
   <si>
-    <t>//main[@class='mb-5']/div/div/div/label[1]</t>
+    <t>//*[text()=' Sale ']</t>
   </si>
   <si>
     <t>ci.PurchaseButton</t>
   </si>
   <si>
-    <t>//main[@class='mb-5']/div/div/div/label[2]</t>
+    <t>//*[text()=' Purchase ']</t>
   </si>
   <si>
     <t>ci.BuyerDetails</t>
@@ -648,7 +648,7 @@
     <t>bd.customer.name</t>
   </si>
   <si>
-    <t>//*[@id='ptd-input-10']</t>
+    <t>(//div[@class='p-2 p-md-3'])[1]/form/div[1]/div/select</t>
   </si>
   <si>
     <t>bd.customer.name.values</t>
@@ -855,7 +855,7 @@
     <t>Item.Name</t>
   </si>
   <si>
-    <t>Fermented</t>
+    <t>Yogurt</t>
   </si>
   <si>
     <t>Qty.enterValue</t>
@@ -1056,7 +1056,37 @@
     <t>view.vouchers.locat</t>
   </si>
   <si>
-    <t>//div[@class='mb-3 clearfix d-print-none']/div/span/button/span[text()='View Vouchers']</t>
+    <t>//*[text()='View Vouchers']</t>
+  </si>
+  <si>
+    <t>receive.payment.button</t>
+  </si>
+  <si>
+    <t>//*[text()='Receive Payment ']</t>
+  </si>
+  <si>
+    <t>click.rectify</t>
+  </si>
+  <si>
+    <t>//*[text()='Rectify']</t>
+  </si>
+  <si>
+    <t>Invoice.edit.heading</t>
+  </si>
+  <si>
+    <t>//*[text()=' Edit Invoice ']</t>
+  </si>
+  <si>
+    <t>click.delete.invoice</t>
+  </si>
+  <si>
+    <t>//*[text()='Cancel']</t>
+  </si>
+  <si>
+    <t>receivePayment.heading</t>
+  </si>
+  <si>
+    <t>//div[@class='modal-content']/div/div/div/b</t>
   </si>
   <si>
     <t>vouchers.visible</t>
@@ -1068,19 +1098,25 @@
     <t>cancel.Invoice</t>
   </si>
   <si>
-    <t>//div[@class='mb-3 clearfix d-print-none']/div/span/button/span[text()='Cancel']</t>
+    <t>//div[@class='container-fluid']/div/div/span/button[2]</t>
   </si>
   <si>
     <t>InvoiceCancel.Button.Table</t>
   </si>
   <si>
-    <t>//*[@id='__BVID__940___BV_modal_content_']</t>
+    <t>//div[@class='modal fade show']/div/div</t>
+  </si>
+  <si>
+    <t>InvoiceCancel.Button.conf.table</t>
+  </si>
+  <si>
+    <t>(//div[@class='modal-content'])[2]/footer/button[text()='Cancel']</t>
   </si>
   <si>
     <t>InvoiceCancel.Button.conf</t>
   </si>
   <si>
-    <t>//*[@id='__BVID__940___BV_modal_footer_']/button[text()='OK']</t>
+    <t>(//div[@class='modal-content'])[2]/footer/button[text()='OK']</t>
   </si>
   <si>
     <t>cancel.pop.message.xpath</t>
@@ -1099,6 +1135,201 @@
   </si>
   <si>
     <t>(//div[@class='card-body'])[4]/table/tbody/tr[1]/td[2]</t>
+  </si>
+  <si>
+    <t>Sales.supplier.button</t>
+  </si>
+  <si>
+    <t>//*[text()='Supplier']</t>
+  </si>
+  <si>
+    <t>bd.supplierName.value</t>
+  </si>
+  <si>
+    <t>VEGAN COCONUT MILK POWDER</t>
+  </si>
+  <si>
+    <t>Supplier.default.values</t>
+  </si>
+  <si>
+    <t>{
+  "inv": {
+    "no": true,
+    "ebn": true,
+    "pin": true,
+    "addr": true,
+    "date": true,
+    "role": true,
+    "class": {
+      "mr-md-1": true,
+      "ml-md-1": true
+    },
+    "state": true,
+    "issuer": true,
+    "delNote": {
+      "no": {
+        "format": {
+          "code": {
+            "in": "DIN",
+            "out": "DOUT"
+          }
+        }
+      }
+    },
+    "supInvNo": true,
+    "supInvDate": true
+  },
+  "bill": {
+    "hsn": true,
+    "qty": {
+      "checkStock": true,
+      "mobileMode": {
+        "disabled": true
+      }
+    },
+    "vat": true,
+    "cess": true,
+    "cgst": true,
+    "fqty": true,
+    "igst": true,
+    "rate": true,
+    "sgst": true,
+    "index": true,
+    "total": {
+      "mobileMode": true
+    },
+    "addBtn": {
+      "mobileMode": true
+    },
+    "footer": {
+      "vat": true,
+      "cess": true,
+      "igst": true,
+      "total": true,
+      "taxable": true,
+      "discount": true
+    },
+    "editBtn": {
+      "mobileMode": true
+    },
+    "product": {
+      "addBtn": true,
+      "mobileMode": {
+        "disabled": true
+      }
+    },
+    "taxable": true,
+    "discount": true
+  },
+  "ship": {
+    "pin": true,
+    "tin": true,
+    "addr": true,
+    "name": true,
+    "class": {
+      "ml-md-1": true
+    },
+    "gstin": true,
+    "state": true,
+    "copyFlag": true
+  },
+  "type": true,
+  "party": {
+    "pin": true,
+    "tin": true,
+    "addr": true,
+    "name": true,
+    "type": true,
+    "class": {
+      "mr-md-1": true
+    },
+    "gstin": true,
+    "state": true,
+    "custid": true,
+    "options": {
+      "gstin": true,
+      "states": true
+    }
+  },
+  "total": {
+    "vat": true,
+    "cess": true,
+    "igst": true,
+    "value": true,
+    "taxable": true,
+    "discount": true,
+    "roundOff": true,
+    "valueText": true
+  },
+  "payment": {
+    "bank": {
+      "no": true,
+      "ifsc": true,
+      "name": true,
+      "branch": true
+    },
+    "mode": true,
+    "class": {
+      "mr-md-1": true
+    }
+  },
+  "taxType": true,
+  "comments": {
+    "class": {
+      "ml-md-1": true
+    }
+  },
+  "transport": {
+    "vno": true,
+    "date": true,
+    "mode": true,
+    "class": {
+      "mr-md-1": true,
+      "ml-md-1": true
+    },
+    "packageCount": true,
+    "reverseCharge": true
+  }
+}</t>
+  </si>
+  <si>
+    <t>select.placeofSupply</t>
+  </si>
+  <si>
+    <t>(//div[@class='p-2 p-md-3'])[2]/div[2]/div[2]/div/select</t>
+  </si>
+  <si>
+    <t>Sales.customer.button</t>
+  </si>
+  <si>
+    <t>//*[text()='Customer']</t>
+  </si>
+  <si>
+    <t>kebabMenu.invoice</t>
+  </si>
+  <si>
+    <t>//div[@class='card-header px-2']/button</t>
+  </si>
+  <si>
+    <t>filter.Invoice</t>
+  </si>
+  <si>
+    <t>//button[@title='Filters']</t>
+  </si>
+  <si>
+    <t>filter.All.checkbox</t>
+  </si>
+  <si>
+    <t>//div[@class='my-2 ml-1']/div/label[text()=' All ']</t>
+  </si>
+  <si>
+    <t>select.purchase</t>
+  </si>
+  <si>
+    <t>select.customer.placeofSupply</t>
+  </si>
+  <si>
+    <t>(//div[@class='p-2 p-md-3'])[2]/div[2]/div[3]/div/select</t>
   </si>
 </sst>
 </file>
@@ -2225,10 +2456,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B209"/>
+  <dimension ref="A1:B215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+      <selection activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -3337,68 +3568,132 @@
       </c>
     </row>
     <row r="138" spans="1:2">
-      <c r="A138" s="4"/>
-      <c r="B138" s="5"/>
+      <c r="A138" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="139" spans="1:2">
-      <c r="A139" s="4"/>
-      <c r="B139" s="5"/>
+      <c r="A139" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="140" spans="1:2">
-      <c r="A140" s="4"/>
-      <c r="B140" s="5"/>
+      <c r="A140" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="141" spans="1:2">
-      <c r="A141" s="4"/>
-      <c r="B141" s="5"/>
+      <c r="A141" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="142" spans="1:2">
-      <c r="A142" s="4"/>
-      <c r="B142" s="5"/>
+      <c r="A142" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="143" spans="1:2">
-      <c r="A143" s="4"/>
-      <c r="B143" s="5"/>
+      <c r="A143" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="144" spans="1:2">
-      <c r="A144" s="4"/>
-      <c r="B144" s="5"/>
+      <c r="A144" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="145" spans="1:2">
-      <c r="A145" s="4"/>
-      <c r="B145" s="5"/>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="4"/>
-      <c r="B146" s="5"/>
+      <c r="A145" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="146" ht="30" customHeight="1" spans="1:2">
+      <c r="A146" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B146" s="8" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="147" spans="1:2">
-      <c r="A147" s="4"/>
-      <c r="B147" s="5"/>
+      <c r="A147" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="148" spans="1:2">
-      <c r="A148" s="4"/>
-      <c r="B148" s="5"/>
+      <c r="A148" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="149" spans="1:2">
-      <c r="A149" s="4"/>
-      <c r="B149" s="5"/>
+      <c r="A149" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="150" spans="1:2">
-      <c r="A150" s="4"/>
-      <c r="B150" s="5"/>
+      <c r="A150" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="151" spans="1:2">
-      <c r="A151" s="4"/>
-      <c r="B151" s="5"/>
+      <c r="A151" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="152" spans="1:2">
-      <c r="A152" s="4"/>
-      <c r="B152" s="5"/>
+      <c r="A152" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="153" spans="1:2">
-      <c r="A153" s="4"/>
-      <c r="B153" s="5"/>
+      <c r="A153" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="4"/>
@@ -3623,6 +3918,30 @@
     <row r="209" spans="1:2">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" s="4"/>
+      <c r="B210" s="5"/>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" s="4"/>
+      <c r="B211" s="5"/>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="4"/>
+      <c r="B212" s="5"/>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="4"/>
+      <c r="B213" s="5"/>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" s="4"/>
+      <c r="B214" s="5"/>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" s="4"/>
+      <c r="B215" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>

</xml_diff>